<commit_message>
con carga masiva de mascotas
</commit_message>
<xml_diff>
--- a/src/assets/excel-templates/massive-load-pets.xlsx
+++ b/src/assets/excel-templates/massive-load-pets.xlsx
@@ -15,6 +15,13 @@
     <sheet name="pets" sheetId="2" r:id="rId1"/>
     <sheet name="references" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Canarios">references!$D$2:$D$4</definedName>
+    <definedName name="Especies">references!$A$2:$A$4</definedName>
+    <definedName name="Gatos">references!$C$2:$C$4</definedName>
+    <definedName name="Perros">references!$B$2:$B$5</definedName>
+    <definedName name="razas">references!$A$2:$A$4</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>petName</t>
   </si>
@@ -50,45 +57,15 @@
     <t>phone</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>gender</t>
   </si>
   <si>
-    <t>Colmena</t>
-  </si>
-  <si>
-    <t>abx</t>
-  </si>
-  <si>
-    <t>Juan López</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>a@aaa.com</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>Rosa Meléndez</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>v@aaa.com</t>
-  </si>
-  <si>
     <t>specie</t>
   </si>
   <si>
@@ -113,28 +90,114 @@
     <t>Schnauzer</t>
   </si>
   <si>
-    <t>Hembra</t>
-  </si>
-  <si>
-    <t>Rocky</t>
-  </si>
-  <si>
-    <t>Macho</t>
-  </si>
-  <si>
     <t>birthday</t>
+  </si>
+  <si>
+    <t>Especies</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Oreja</t>
+  </si>
+  <si>
+    <t>Guapo</t>
+  </si>
+  <si>
+    <t>Luna</t>
+  </si>
+  <si>
+    <t>Chino</t>
+  </si>
+  <si>
+    <t>Piojo</t>
+  </si>
+  <si>
+    <t>Persa</t>
+  </si>
+  <si>
+    <t>Gloster</t>
+  </si>
+  <si>
+    <t>Roller</t>
+  </si>
+  <si>
+    <t>Harzer Roller</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>brisa_love</t>
+  </si>
+  <si>
+    <t>migueloncho</t>
+  </si>
+  <si>
+    <t>jurgen01</t>
+  </si>
+  <si>
+    <t>karla_keith</t>
+  </si>
+  <si>
+    <t>andreita_lopez</t>
+  </si>
+  <si>
+    <t>Brisa Castillo Lezama</t>
+  </si>
+  <si>
+    <t>Miguel Diaz Montes</t>
+  </si>
+  <si>
+    <t>Karla Silva Medina</t>
+  </si>
+  <si>
+    <t>Andrea Sifuentes López</t>
+  </si>
+  <si>
+    <t>bribri@petso.org</t>
+  </si>
+  <si>
+    <t>migueloncho@petso.org</t>
+  </si>
+  <si>
+    <t>jauregui.jorge@petso.org</t>
+  </si>
+  <si>
+    <t>karla.silva@petso.org</t>
+  </si>
+  <si>
+    <t>andreita.sl@petso.org</t>
+  </si>
+  <si>
+    <t>Jorge Jimenez Gonzalez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -178,18 +241,33 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -466,242 +544,370 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11" style="1"/>
-    <col min="3" max="3" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11" style="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="1"/>
+    <col min="1" max="2" width="11" style="3"/>
+    <col min="3" max="3" width="19.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" style="3"/>
+    <col min="6" max="6" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E2" s="8">
+        <v>44433</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="G2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="3">
+        <v>963001001</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E3" s="8">
+        <v>44433</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="3">
+        <v>963001001</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8">
+        <v>44433</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3">
+        <v>964470073</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="6">
-        <v>45529</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1">
-        <v>88554477</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="D5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8">
+        <v>44433</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="3">
+        <v>963258961</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="D6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="8">
+        <v>44433</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="3">
+        <v>987414785</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="6">
-        <v>45481</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1">
-        <v>88552244</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="10:10">
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="10:10">
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="10:10">
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="10:10">
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="10:10">
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="10:10">
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="10:10">
-      <c r="J23" s="2"/>
+      <c r="C7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8">
+        <v>44433</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="3">
+        <v>963214565</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="9:9">
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="9:9">
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="9:9">
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="9:9">
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="9:9">
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="9:9">
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="9:9">
+      <c r="I23" s="9"/>
     </row>
   </sheetData>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3">
+      <formula1>Especies</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C7">
+      <formula1>INDIRECT(B2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="J3:J23" r:id="rId1" display="v@aaa.com"/>
-    <hyperlink ref="J2" r:id="rId2"/>
-    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3:I7" r:id="rId2" display="bribri@petso.org"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" s="3" t="s">
-        <v>25</v>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>